<commit_message>
all-in-one template tutorial updated
</commit_message>
<xml_diff>
--- a/GitHubPages/documents/All_In_One_Template_Example.xlsx
+++ b/GitHubPages/documents/All_In_One_Template_Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stations" sheetId="2" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>Farmer 2</t>
   </si>
   <si>
-    <t>Yoghurt Factory</t>
-  </si>
-  <si>
     <t>Producer</t>
   </si>
   <si>
@@ -245,7 +242,10 @@
     <t>jars</t>
   </si>
   <si>
-    <t>Yoghurt</t>
+    <t>Yogurt Factory</t>
+  </si>
+  <si>
+    <t>Yogurt</t>
   </si>
 </sst>
 </file>
@@ -442,6 +442,38 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -474,62 +506,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -837,7 +837,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,31 +859,31 @@
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="6" t="s">
@@ -906,16 +906,16 @@
         <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1">
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>33</v>
@@ -932,16 +932,16 @@
         <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1">
         <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>33</v>
@@ -952,106 +952,106 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1">
         <v>67</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="1">
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,125 +1093,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="25" t="s">
+      <c r="D1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="29" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="25" t="s">
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="26"/>
-      <c r="O1" s="16" t="s">
+      <c r="N1" s="27"/>
+      <c r="O1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="T1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="12"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
     </row>
     <row r="2" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="30" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="N2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="17"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -1235,24 +1235,24 @@
         <v>1500</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="G4" s="1">
         <v>2</v>
@@ -1276,24 +1276,24 @@
         <v>1200</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>
@@ -1317,24 +1317,24 @@
         <v>1300</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="1">
         <v>4</v>
@@ -1358,24 +1358,24 @@
         <v>1000</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="1">
         <v>4</v>
@@ -1399,24 +1399,24 @@
         <v>300</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G8" s="1">
         <v>5</v>
@@ -1440,24 +1440,24 @@
         <v>1200</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G9" s="1">
         <v>5</v>
@@ -1481,10 +1481,10 @@
         <v>1000</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1520,9 +1520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1540,50 +1538,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>